<commit_message>
Cambios al código en python, Arduino Uno y MEGA, con carpeta de Proyecto completo
</commit_message>
<xml_diff>
--- a/Tercer avance y final/Control_Acceso.xlsx
+++ b/Tercer avance y final/Control_Acceso.xlsx
@@ -401,10 +401,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" outlineLevelCol="0"/>
@@ -542,6 +542,77 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>D9A6F651</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Manuel Erices</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>20432608-8</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>E9447748</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>Juan Pérez</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>12345678-9</t>
+        </is>
+      </c>
+      <c r="D7" s="3" t="inlineStr">
+        <is>
+          <t>sí</t>
+        </is>
+      </c>
+      <c r="E7" s="3" t="inlineStr">
+        <is>
+          <t>Entrada</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>E9447748</t>
+        </is>
+      </c>
+      <c r="B8" s="3" t="inlineStr">
+        <is>
+          <t>Juan Pérez</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>12345678-9</t>
+        </is>
+      </c>
+      <c r="D8" s="3" t="inlineStr">
+        <is>
+          <t>sí</t>
+        </is>
+      </c>
+      <c r="E8" s="3" t="inlineStr">
+        <is>
+          <t>Salida</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9" horizontalDpi="1200" verticalDpi="1200"/>
@@ -554,9 +625,9 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:F83"/>
+  <dimension ref="A2:F118"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A86" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1962,6 +2033,621 @@
         </is>
       </c>
     </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>334914AC</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:39:59</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Entrada</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>334914AC</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:40:20</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Entrada</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>334914AC</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:40:44</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Entrada</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>334914AC</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:40:55</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Salida</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>334914AC</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:41:17</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Entrada</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>334914AC</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:41:27</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Salida</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>334914AC</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:46:15</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Entrada</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>334914AC</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:46:26</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Salida</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>334914AC</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:54:42</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Entrada</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>334914AC</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:54:51</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Salida</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>334914AC</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:13:20</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Entrada</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>334914AC</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:14:38</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Entrada</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>334914AC</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:15:02</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Entrada</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>334914AC</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:15:16</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Entrada</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>334914AC</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:17:04</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Entrada</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>334914AC</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:17:25</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Entrada</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>334914AC</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:18:03</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Entrada</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>334914AC</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:18:13</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Salida</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>334914AC</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:31:46</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>Entrada</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>334914AC</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:32:17</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>Entrada</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>334914AC</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:32:26</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>Salida</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>334914AC</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:33:12</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>Entrada</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>334914AC</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:33:46</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>Entrada</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>334914AC</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:33:55</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>Salida</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>D9A6F651</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>2024-12-03 14:02:03</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>Entrada</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>Acceso autorizado</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>D9A6F651</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>2024-12-03 14:02:12</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>Entrada</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>Acceso autorizado</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>D9A6F651</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>2024-12-03 14:02:12</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>Entrada</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>Acceso autorizado</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>D9A6F651</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>2024-12-03 14:02:12</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>Entrada</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>Acceso autorizado</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>3DD64D4C</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:03:46</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>Entrada</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>3DD64D4C</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:03:59</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>Salida</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>E9447748</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:07:37</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>Entrada</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>E9447748</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:07:50</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>Salida</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>E9447748</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:09:10</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>Entrada</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>E9447748</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:09:20</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>Salida</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>334914AC</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:22:43</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>Entrada</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1973,9 +2659,9 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:C163"/>
+  <dimension ref="A2:C595"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A524" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -3119,6 +3805,3030 @@
         </is>
       </c>
     </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:39:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:39:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:39:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:39:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:39:51</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:46:46</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:55:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:55:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:57:19</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:57:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:57:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:57:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:57:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:57:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:57:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:57:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:57:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:57:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:57:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:57:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:57:52</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:57:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:57:56</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:57:58</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:58:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:58:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:58:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:58:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:58:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:58:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:58:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:58:18</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:58:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:58:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:58:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:58:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:58:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:58:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:58:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:58:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:58:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:58:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:58:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:58:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:58:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:58:52</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:58:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:58:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:59:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:59:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:59:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:59:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:59:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:59:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:59:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:59:19</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:59:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:59:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:59:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:59:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:59:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:59:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:59:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:59:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:59:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:59:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:59:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:59:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:59:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:59:51</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:59:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:59:56</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>2024-12-03 11:59:58</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:00:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:00:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:00:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:00:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:00:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:00:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:00:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:00:19</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:00:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:00:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:00:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:00:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:00:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:00:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:00:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:00:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:00:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:00:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:00:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:00:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:00:51</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:00:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:00:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:00:58</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:01:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:01:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:01:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:01:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:01:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:01:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:01:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:01:18</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:01:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:01:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:01:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:01:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:01:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:01:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:01:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:01:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:01:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:01:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:01:51</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:01:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:01:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:01:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:02:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:02:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:02:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:02:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:02:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:02:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:02:18</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:02:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:02:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:02:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:02:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:02:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:02:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:02:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:02:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:02:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:02:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:02:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:02:52</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:02:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:02:58</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:03:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:03:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:03:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:03:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:03:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:03:19</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:03:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:03:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:03:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:03:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:03:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:03:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:03:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:03:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:03:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:03:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:03:52</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:03:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:03:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:03:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:04:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:04:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:04:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:04:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:04:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:04:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:04:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:04:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:04:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:04:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:04:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:04:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:04:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:04:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:04:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:04:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:04:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:04:51</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:04:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:05:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:05:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:05:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:05:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:05:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:05:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:05:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:05:18</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:05:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:05:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:05:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:05:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:05:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:05:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:05:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:05:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:05:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:05:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:05:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:05:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:05:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:05:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:05:51</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:05:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:05:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:05:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:06:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:06:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:06:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:06:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:06:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:06:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:06:19</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:06:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:06:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:06:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:06:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:06:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:06:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:06:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:06:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:06:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:06:46</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:06:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:06:52</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:06:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:06:56</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:06:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:07:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:07:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:07:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:07:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:07:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:07:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:07:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:07:19</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:07:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:07:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:07:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:07:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:07:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:07:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:07:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:07:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:07:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:07:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:07:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:07:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:07:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:07:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:07:52</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:07:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:07:58</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:08:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:08:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:08:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:08:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:08:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:08:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:08:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:08:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:08:18</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:08:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:08:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:08:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:08:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:08:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:08:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:08:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:08:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:08:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:08:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:08:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:08:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:08:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:08:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:08:52</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:08:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:08:56</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:08:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:09:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:09:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:09:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:09:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:09:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:09:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:09:19</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:09:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:09:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:09:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:09:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:09:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:09:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:09:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:09:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:09:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:09:51</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:09:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:09:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:09:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:10:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:10:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:10:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:10:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:10:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:10:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:10:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:10:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:10:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:10:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:10:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:10:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:10:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:10:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:10:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:10:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:10:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:10:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:10:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:10:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:10:51</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:10:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:11:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:11:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:11:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:11:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:11:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:11:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:11:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:11:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:11:18</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:11:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:11:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:11:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:11:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:11:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:11:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:11:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:11:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:11:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:11:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:11:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:11:46</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:11:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:11:51</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:11:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:11:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:11:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:12:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:12:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:12:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:12:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:12:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:12:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:12:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:12:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:12:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:12:19</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:12:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:12:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:12:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:12:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:12:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:12:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:12:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:12:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:12:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:12:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:12:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:12:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:12:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:12:51</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:12:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:12:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:12:58</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:13:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:13:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:13:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:13:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:13:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:13:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:13:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:13:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:03:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:03:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:03:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:07:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:33:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:33:52</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:33:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:33:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:33:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:34:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:34:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:35:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:35:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:35:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:35:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:35:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:35:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:35:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:35:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:35:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:35:48</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:35:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:36:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:36:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:36:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:36:18</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:36:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:36:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:36:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:36:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:36:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:36:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:36:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:37:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:37:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:37:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:37:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:37:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:37:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:37:18</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:37:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:37:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:37:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:37:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:37:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:37:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>2024-12-04 16:37:41</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>